<commit_message>
Edited the result excel files
</commit_message>
<xml_diff>
--- a/report/sort algorithms Extended.xlsx
+++ b/report/sort algorithms Extended.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\OneDrive\Documents\my_projects\CS15 Sorting Algorithms\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A111C7A0-B3A3-4D48-8C61-C4D1DB7E983F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B372E5B1-E50C-4550-962C-1CD3CE6472C8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10290" yWindow="1725" windowWidth="28800" windowHeight="11505" xr2:uid="{B2EC1B3E-C2AC-4CD1-8DF7-1604AC6E84AB}"/>
+    <workbookView xWindow="3510" yWindow="2745" windowWidth="28800" windowHeight="11505" xr2:uid="{B2EC1B3E-C2AC-4CD1-8DF7-1604AC6E84AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -129,13 +129,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>InsertionSort</a:t>
+              <a:t>InsertionSort and Heapsort runtime</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> and Heapsort runtime</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -152,7 +147,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -189,7 +184,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -198,7 +193,20 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -306,7 +314,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -315,7 +323,20 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -416,6 +437,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="1130411471"/>
         <c:axId val="909967967"/>
@@ -427,6 +449,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -449,7 +485,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -478,20 +514,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -499,7 +521,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -531,7 +553,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -553,8 +575,14 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -589,14 +617,13 @@
         <c:showKeys val="1"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9525">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
                 <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -635,7 +662,7 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="lt1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -707,7 +734,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -718,7 +745,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -741,18 +768,18 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="bg1"/>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -764,7 +791,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -772,11 +799,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -808,12 +835,12 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -823,12 +850,12 @@
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -840,13 +867,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -858,12 +885,12 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -873,18 +900,19 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -906,15 +934,13 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -929,10 +955,46 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -940,67 +1002,128 @@
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1013,54 +1136,17 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -1070,8 +1156,8 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
+  </cs:seriesLine>
+  <cs:title>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1081,66 +1167,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1149,14 +1176,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1170,7 +1197,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
@@ -1186,8 +1213,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1203,6 +1230,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1210,14 +1248,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1578,7 +1610,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>